<commit_message>
Finalisation du burndown chart
</commit_message>
<xml_diff>
--- a/BurndownChart.xlsx
+++ b/BurndownChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\306-Projet-RealiserPetitProjet\FAT-306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5-repertoires-ict-ssd\PROJETS\Wak\FAT-306\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
     <t>Courbe de prévision</t>
   </si>
   <si>
-    <t xml:space="preserve">Courbe de </t>
+    <t>Courbe réelle</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Courbe de </c:v>
+                  <c:v>Courbe réelle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -332,6 +332,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -363,6 +372,31 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>Périodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -1186,16 +1220,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1483,7 +1517,7 @@
   <dimension ref="B4:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,6 +1590,9 @@
       <c r="F9">
         <v>6</v>
       </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10">
@@ -1564,6 +1601,9 @@
       <c r="F10">
         <v>3</v>
       </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E11">
@@ -1571,6 +1611,9 @@
       </c>
       <c r="F11">
         <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>